<commit_message>
added the list of modules
</commit_message>
<xml_diff>
--- a/DIAGRAMS/MODULE-LIST.xlsx
+++ b/DIAGRAMS/MODULE-LIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc Jimenez\Documents\GitHub\SOFTDEV-QUALITY\DIAGRAMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92F485B6-E38D-418D-BAE1-06132B27873B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59851A51-83E5-44B2-AA70-33D7AC29ED0F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15276" windowHeight="3972" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Module Name</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>3.1. Fill-up information</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -547,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,7 +714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="8" t="s">
         <v>48</v>
@@ -720,7 +723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="4" t="s">
         <v>8</v>
@@ -729,7 +732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="8" t="s">
         <v>49</v>
@@ -738,7 +741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="4" t="s">
         <v>9</v>
@@ -747,7 +750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>12</v>
       </c>
@@ -758,7 +761,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="8" t="s">
         <v>50</v>
@@ -767,7 +770,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="4" t="s">
         <v>14</v>
@@ -776,7 +779,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="4" t="s">
         <v>16</v>
@@ -785,7 +788,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="8" t="s">
         <v>53</v>
@@ -794,43 +797,46 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="4" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
quick rest -- will continue laterz
</commit_message>
<xml_diff>
--- a/DIAGRAMS/MODULE-LIST.xlsx
+++ b/DIAGRAMS/MODULE-LIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc Jimenez\Documents\GitHub\SOFTDEV-QUALITY\DIAGRAMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44C5ACD-D9CC-4437-B6E8-2AD43952011C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A15AC0F-9A2E-434C-BA39-23B0A7CF2F66}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15276" windowHeight="3972" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="177">
   <si>
     <t>Module Name</t>
   </si>
@@ -85,9 +85,6 @@
     <t>5.0. Create Resource</t>
   </si>
   <si>
-    <t>6.0. View Resourve</t>
-  </si>
-  <si>
     <t>7.0. Edit Resource</t>
   </si>
   <si>
@@ -209,13 +206,7 @@
     <t>5.1.1.1.6. Select "Hygiene" Category</t>
   </si>
   <si>
-    <t>5.1.1.1.7. Select "Defense" Category</t>
-  </si>
-  <si>
     <t>5.1.2. Select Supply Category</t>
-  </si>
-  <si>
-    <t>5.1.2.1. Select Equipment Category</t>
   </si>
   <si>
     <t>5.1.2.1.1. Select "Houseware" Category</t>
@@ -646,12 +637,108 @@
     <t>Regional Admin
 Provincial Admin</t>
   </si>
+  <si>
+    <t>The supplier can be deactivated rather than be deleted to still keep an intact record of all suppliers in the system</t>
+  </si>
+  <si>
+    <t>A resource can be created, wherein it can either be an Equipment (which is permanent or lasts longer) or a Supply (which is easily used up)</t>
+  </si>
+  <si>
+    <t>The user can select what type of resource it is (either Equipment or Supply)</t>
+  </si>
+  <si>
+    <t>A equipment resource will be created, along with the basic information needed for it.</t>
+  </si>
+  <si>
+    <t>If equipment is chosen, there will be a total of 7 equipment categories to sort the item into.</t>
+  </si>
+  <si>
+    <t>An electrical item will be created. Electrical items consists of Extension Cords, Wires, Routers, etc.</t>
+  </si>
+  <si>
+    <t>A construction item will be created. Construction items consists of Jackhammers, Shovels, Pliers, etc.; Items typically used for Clearing Operations</t>
+  </si>
+  <si>
+    <t>A defense item will be created. Survival items consists of Barricades, Handcuffs, etc; Items typically used by the Protection cluster</t>
+  </si>
+  <si>
+    <t>A survival item will be created. Survival items consists of safety ropes, Torches, Pulleys, Oxygen Tanks, etc; Items typically used for Search and Rescue operations</t>
+  </si>
+  <si>
+    <t>A medical item will be created. Medical items consists of Nebulizers, Thermometers, Scalpels, etc.</t>
+  </si>
+  <si>
+    <t>5.1.1.1.7. Select "Others" Category</t>
+  </si>
+  <si>
+    <t>A hygiene item will be created. Hygiene items consists of Water Containers, Portalets, Floor Mops, etc; Items typically used by the WaSH (Water, Sanitation, and Heath) cluster</t>
+  </si>
+  <si>
+    <t>All items under this category are those cannot be categorized in any of the aforementioned categories</t>
+  </si>
+  <si>
+    <t>A supply resource will be created, along with the basic information needed for it.</t>
+  </si>
+  <si>
+    <t>5.1.2.1. Select Supply Category</t>
+  </si>
+  <si>
+    <t>If supply is chosen, there will be a total of 13 supply categories to sort the item into.</t>
+  </si>
+  <si>
+    <t>A houseware supply will be created. Hygiene items consists of Water Containers, Portalets, Floor Mops, etc.</t>
+  </si>
+  <si>
+    <t>&lt;-- ilipat sa Equipment??</t>
+  </si>
+  <si>
+    <t>A Clothing/Textile supply will be created.</t>
+  </si>
+  <si>
+    <t>A Food Item supply will be created.</t>
+  </si>
+  <si>
+    <t>A Sleeping Gear supply will be created.</t>
+  </si>
+  <si>
+    <t>A Construction Material supply will be created. Examples of these are cement sacks, Steel bars, etc.</t>
+  </si>
+  <si>
+    <t>An Agriculture supply will be created. Examples of these are seedlings, soil, etc.</t>
+  </si>
+  <si>
+    <t>A Medical supply will be created. Examples of these are medicine, ointments, etc.</t>
+  </si>
+  <si>
+    <t>An Electrical supply will be created. Examples of these are seedlings, soil, etc.</t>
+  </si>
+  <si>
+    <t>A Vehicle Supply will be created. Examples of these are Fuel, Machine Oil, etc.</t>
+  </si>
+  <si>
+    <t>An Education Supply will be created. Examples of these are Paper, Pens, Crayons, etc.</t>
+  </si>
+  <si>
+    <t>A Survival Supply will be created. Examples of these are Saline Tabs, Soap, etc.</t>
+  </si>
+  <si>
+    <t>Those supplies that cannot be categorized to the aforementions categories, will be placed here.</t>
+  </si>
+  <si>
+    <t>A WaSH Supply will be created. Examples of these are Water Purification Tablets, Potable Water, Soap, etc.</t>
+  </si>
+  <si>
+    <t>Other requirements for the Resource will be inputted in this process</t>
+  </si>
+  <si>
+    <t>6.0. View Resource</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,6 +750,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -691,7 +785,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -700,7 +794,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -713,11 +818,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -746,12 +852,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+  <cellStyles count="3">
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1030,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C53" activeCellId="1" sqref="C58 C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1041,6 +1161,7 @@
     <col min="1" max="1" width="25.44140625" customWidth="1"/>
     <col min="2" max="2" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="25.44140625" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1054,7 +1175,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>2</v>
@@ -1068,10 +1189,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>11</v>
@@ -1080,13 +1201,13 @@
     <row r="3" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>10</v>
@@ -1095,13 +1216,13 @@
     <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>10</v>
@@ -1110,13 +1231,13 @@
     <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>10</v>
@@ -1125,13 +1246,13 @@
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>10</v>
@@ -1140,13 +1261,13 @@
     <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>10</v>
@@ -1155,13 +1276,13 @@
     <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>10</v>
@@ -1170,13 +1291,13 @@
     <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>11</v>
@@ -1188,10 +1309,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>10</v>
@@ -1200,13 +1321,13 @@
     <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>10</v>
@@ -1215,13 +1336,13 @@
     <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>10</v>
@@ -1233,10 +1354,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>10</v>
@@ -1245,13 +1366,13 @@
     <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>10</v>
@@ -1260,13 +1381,13 @@
     <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>10</v>
@@ -1275,13 +1396,13 @@
     <row r="16" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>10</v>
@@ -1290,13 +1411,13 @@
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>10</v>
@@ -1308,10 +1429,10 @@
         <v>8</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>11</v>
@@ -1320,13 +1441,13 @@
     <row r="19" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>11</v>
@@ -1338,10 +1459,10 @@
         <v>9</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>10</v>
@@ -1355,28 +1476,28 @@
         <v>13</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1385,13 +1506,13 @@
         <v>14</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -1400,42 +1521,46 @@
         <v>16</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="D25" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="D26" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E26" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" t="s">
         <v>47</v>
-      </c>
-      <c r="F26" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -1443,885 +1568,943 @@
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="D27" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="6"/>
+        <v>48</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="D28" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="D29" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
       <c r="B30" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>149</v>
+      </c>
       <c r="D30" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
       <c r="B31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="D31" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="6"/>
+        <v>52</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>153</v>
+      </c>
       <c r="D32" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="D33" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="6"/>
+        <v>54</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>152</v>
+      </c>
       <c r="D34" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>154</v>
+      </c>
       <c r="D35" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>156</v>
+      </c>
       <c r="D36" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="6"/>
+        <v>155</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>157</v>
+      </c>
       <c r="D37" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="6"/>
+        <v>57</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>158</v>
+      </c>
       <c r="D38" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="6"/>
+        <v>159</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>160</v>
+      </c>
       <c r="D39" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
-      <c r="B40" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B40" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
       <c r="B41" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" s="6"/>
+        <v>59</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>164</v>
+      </c>
       <c r="D41" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="B42" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>163</v>
+      </c>
       <c r="D42" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C43" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>165</v>
+      </c>
       <c r="D43" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>166</v>
+      </c>
       <c r="D44" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C45" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>167</v>
+      </c>
       <c r="D45" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
       <c r="B46" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>168</v>
+      </c>
       <c r="D46" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="9"/>
       <c r="B47" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" s="6"/>
+        <v>65</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>169</v>
+      </c>
       <c r="D47" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="9"/>
       <c r="B48" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C48" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>170</v>
+      </c>
       <c r="D48" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="9"/>
       <c r="B49" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" s="6"/>
+        <v>67</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>171</v>
+      </c>
       <c r="D49" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A50" s="9"/>
       <c r="B50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="9"/>
       <c r="B51" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>172</v>
+      </c>
       <c r="D51" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>173</v>
+      </c>
       <c r="D52" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
       <c r="B53" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="6"/>
+        <v>72</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="D53" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A54" s="9"/>
       <c r="B54" s="1" t="s">
-        <v>18</v>
+        <v>176</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
       <c r="B55" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
       <c r="B56" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="9"/>
       <c r="B57" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A58" s="9"/>
       <c r="B58" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C58" s="6"/>
       <c r="D58" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A59" s="9"/>
       <c r="B59" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="B60" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" s="9"/>
       <c r="B61" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
       <c r="B62" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C62" s="6"/>
       <c r="D62" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="9"/>
       <c r="B63" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C63" s="6"/>
       <c r="D63" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="9"/>
       <c r="B64" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C64" s="6"/>
       <c r="D64" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C65" s="6"/>
       <c r="D65" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
       <c r="B66" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="9"/>
       <c r="B67" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="9"/>
       <c r="B68" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="9"/>
       <c r="B69" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="9"/>
       <c r="B70" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C70" s="6"/>
       <c r="D70" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
       <c r="B71" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" s="9"/>
       <c r="B72" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C72" s="6"/>
       <c r="D72" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" s="9"/>
       <c r="B73" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="9"/>
       <c r="B74" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="9"/>
       <c r="B75" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="9"/>
       <c r="B76" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C76" s="6"/>
       <c r="D76" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="9"/>
       <c r="B77" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C77" s="6"/>
       <c r="D77" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78" s="9"/>
       <c r="B78" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A79" s="9"/>
       <c r="B79" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C79" s="6"/>
       <c r="D79" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" s="9"/>
       <c r="B80" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" s="9"/>
       <c r="B81" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C81" s="6"/>
       <c r="D81" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="9"/>
       <c r="B82" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="9"/>
       <c r="B83" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="9"/>
       <c r="B84" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="9"/>
       <c r="B85" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C85" s="6"/>
       <c r="D85" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" s="9"/>
       <c r="B86" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C86" s="6"/>
       <c r="D86" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="9"/>
       <c r="B87" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="9"/>
       <c r="B88" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C88" s="6"/>
       <c r="D88" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="9"/>
       <c r="B89" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C89" s="6"/>
       <c r="D89" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="9"/>
       <c r="B90" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C90" s="6"/>
       <c r="D90" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="9"/>
       <c r="B91" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C91" s="6"/>
       <c r="D91" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="9"/>
       <c r="B92" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C92" s="6"/>
       <c r="D92" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A93" s="9"/>
       <c r="B93" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C93" s="6"/>
       <c r="D93" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A94" s="9"/>
       <c r="B94" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C94" s="6"/>
       <c r="D94" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(( some changes ))
</commit_message>
<xml_diff>
--- a/DIAGRAMS/MODULE-LIST.xlsx
+++ b/DIAGRAMS/MODULE-LIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc Jimenez\Documents\GitHub\SOFTDEV-QUALITY\DIAGRAMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A15AC0F-9A2E-434C-BA39-23B0A7CF2F66}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B70893-364A-46D0-AB90-4095425B4C7A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15276" windowHeight="3972" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -846,12 +846,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -867,6 +861,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1152,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C53" activeCellId="1" sqref="C58 C53"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1165,24 +1165,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1199,7 +1199,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="3" t="s">
         <v>32</v>
       </c>
@@ -1214,7 +1214,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1229,7 +1229,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1244,7 +1244,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="2" t="s">
         <v>118</v>
       </c>
@@ -1259,7 +1259,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
@@ -1274,7 +1274,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="4" t="s">
         <v>36</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
         <v>37</v>
       </c>
@@ -1304,7 +1304,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1319,7 +1319,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="3" t="s">
         <v>38</v>
       </c>
@@ -1334,7 +1334,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
@@ -1349,7 +1349,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1364,7 +1364,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
@@ -1379,7 +1379,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="3" t="s">
         <v>41</v>
       </c>
@@ -1394,7 +1394,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="3" t="s">
         <v>140</v>
       </c>
@@ -1409,7 +1409,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="3" t="s">
         <v>42</v>
       </c>
@@ -1424,7 +1424,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1439,7 +1439,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>43</v>
       </c>
@@ -1454,7 +1454,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1469,7 +1469,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1486,7 +1486,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="3" t="s">
         <v>44</v>
       </c>
@@ -1501,7 +1501,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
@@ -1516,7 +1516,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
@@ -1531,7 +1531,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="3" t="s">
         <v>89</v>
       </c>
@@ -1546,7 +1546,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
@@ -1564,7 +1564,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
@@ -1579,7 +1579,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="3" t="s">
         <v>48</v>
       </c>
@@ -1594,7 +1594,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="2" t="s">
         <v>49</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="4" t="s">
         <v>50</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="5" t="s">
         <v>51</v>
       </c>
@@ -1639,7 +1639,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="5" t="s">
         <v>52</v>
       </c>
@@ -1654,7 +1654,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="5" t="s">
         <v>53</v>
       </c>
@@ -1669,7 +1669,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="5" t="s">
         <v>54</v>
       </c>
@@ -1684,7 +1684,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="5" t="s">
         <v>55</v>
       </c>
@@ -1699,7 +1699,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="5" t="s">
         <v>56</v>
       </c>
@@ -1714,7 +1714,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="5" t="s">
         <v>155</v>
       </c>
@@ -1729,7 +1729,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="2" t="s">
         <v>57</v>
       </c>
@@ -1744,7 +1744,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="4" t="s">
         <v>159</v>
       </c>
@@ -1759,30 +1759,30 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
-      <c r="B40" s="11" t="s">
+      <c r="A40" s="15"/>
+      <c r="B40" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="E40" s="12" t="s">
+      <c r="D40" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="G40" s="14"/>
+      <c r="G40" s="12"/>
     </row>
     <row r="41" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="11" t="s">
         <v>164</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -1793,11 +1793,11 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="9"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="11" t="s">
         <v>163</v>
       </c>
       <c r="D42" s="6" t="s">
@@ -1808,11 +1808,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="9"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="11" t="s">
         <v>165</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -1823,11 +1823,11 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="9"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="11" t="s">
         <v>166</v>
       </c>
       <c r="D44" s="6" t="s">
@@ -1838,11 +1838,11 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="9"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="11" t="s">
         <v>167</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -1853,11 +1853,11 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="9"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="11" t="s">
         <v>168</v>
       </c>
       <c r="D46" s="6" t="s">
@@ -1868,11 +1868,11 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="9"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="11" t="s">
         <v>169</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -1883,11 +1883,11 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="9"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="11" t="s">
         <v>170</v>
       </c>
       <c r="D48" s="6" t="s">
@@ -1898,11 +1898,11 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="11" t="s">
         <v>171</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -1913,11 +1913,11 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A50" s="9"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="11" t="s">
         <v>174</v>
       </c>
       <c r="D50" s="6" t="s">
@@ -1928,11 +1928,11 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="9"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="11" t="s">
         <v>172</v>
       </c>
       <c r="D51" s="6" t="s">
@@ -1943,11 +1943,11 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="9"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="11" t="s">
         <v>173</v>
       </c>
       <c r="D52" s="6" t="s">
@@ -1958,7 +1958,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A53" s="9"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="2" t="s">
         <v>72</v>
       </c>
@@ -1973,7 +1973,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="9"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="1" t="s">
         <v>176</v>
       </c>
@@ -1986,7 +1986,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A55" s="9"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="1" t="s">
         <v>18</v>
       </c>
@@ -1999,7 +1999,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A56" s="9"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="3" t="s">
         <v>88</v>
       </c>
@@ -2012,7 +2012,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="9"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="1" t="s">
         <v>19</v>
       </c>
@@ -2025,7 +2025,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="9"/>
+      <c r="A58" s="15"/>
       <c r="B58" s="1" t="s">
         <v>20</v>
       </c>
@@ -2038,7 +2038,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="9"/>
+      <c r="A59" s="15"/>
       <c r="B59" s="3" t="s">
         <v>73</v>
       </c>
@@ -2051,7 +2051,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="9"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="1" t="s">
         <v>21</v>
       </c>
@@ -2064,7 +2064,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A61" s="9"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="3" t="s">
         <v>74</v>
       </c>
@@ -2077,7 +2077,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A62" s="9"/>
+      <c r="A62" s="15"/>
       <c r="B62" s="3" t="s">
         <v>75</v>
       </c>
@@ -2090,7 +2090,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A63" s="9"/>
+      <c r="A63" s="15"/>
       <c r="B63" s="3" t="s">
         <v>76</v>
       </c>
@@ -2103,7 +2103,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="9"/>
+      <c r="A64" s="15"/>
       <c r="B64" s="1" t="s">
         <v>22</v>
       </c>
@@ -2116,7 +2116,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A65" s="9" t="s">
+      <c r="A65" s="15" t="s">
         <v>77</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2131,7 +2131,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A66" s="9"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="3" t="s">
         <v>78</v>
       </c>
@@ -2144,7 +2144,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A67" s="9"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="2" t="s">
         <v>79</v>
       </c>
@@ -2157,7 +2157,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="9"/>
+      <c r="A68" s="15"/>
       <c r="B68" s="2" t="s">
         <v>80</v>
       </c>
@@ -2170,7 +2170,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
+      <c r="A69" s="15"/>
       <c r="B69" s="2" t="s">
         <v>81</v>
       </c>
@@ -2183,7 +2183,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="9"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="3" t="s">
         <v>85</v>
       </c>
@@ -2196,7 +2196,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="9"/>
+      <c r="A71" s="15"/>
       <c r="B71" s="2" t="s">
         <v>82</v>
       </c>
@@ -2209,7 +2209,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A72" s="9"/>
+      <c r="A72" s="15"/>
       <c r="B72" s="2" t="s">
         <v>83</v>
       </c>
@@ -2222,7 +2222,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="9"/>
+      <c r="A73" s="15"/>
       <c r="B73" s="2" t="s">
         <v>84</v>
       </c>
@@ -2235,7 +2235,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="9"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="3" t="s">
         <v>86</v>
       </c>
@@ -2248,7 +2248,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="9"/>
+      <c r="A75" s="15"/>
       <c r="B75" s="1" t="s">
         <v>24</v>
       </c>
@@ -2261,7 +2261,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="9"/>
+      <c r="A76" s="15"/>
       <c r="B76" s="3" t="s">
         <v>87</v>
       </c>
@@ -2274,7 +2274,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="9"/>
+      <c r="A77" s="15"/>
       <c r="B77" s="1" t="s">
         <v>25</v>
       </c>
@@ -2287,7 +2287,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A78" s="9"/>
+      <c r="A78" s="15"/>
       <c r="B78" s="1" t="s">
         <v>26</v>
       </c>
@@ -2300,7 +2300,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A79" s="9"/>
+      <c r="A79" s="15"/>
       <c r="B79" s="1" t="s">
         <v>27</v>
       </c>
@@ -2313,7 +2313,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A80" s="9"/>
+      <c r="A80" s="15"/>
       <c r="B80" s="3" t="s">
         <v>90</v>
       </c>
@@ -2326,7 +2326,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A81" s="9"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="1" t="s">
         <v>28</v>
       </c>
@@ -2339,7 +2339,7 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A82" s="9"/>
+      <c r="A82" s="15"/>
       <c r="B82" s="3" t="s">
         <v>91</v>
       </c>
@@ -2352,7 +2352,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="9"/>
+      <c r="A83" s="15"/>
       <c r="B83" s="3" t="s">
         <v>93</v>
       </c>
@@ -2365,7 +2365,7 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A84" s="9"/>
+      <c r="A84" s="15"/>
       <c r="B84" s="3" t="s">
         <v>92</v>
       </c>
@@ -2378,7 +2378,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="9"/>
+      <c r="A85" s="15"/>
       <c r="B85" s="1" t="s">
         <v>29</v>
       </c>
@@ -2391,7 +2391,7 @@
       </c>
     </row>
     <row r="86" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A86" s="9"/>
+      <c r="A86" s="15"/>
       <c r="B86" s="1" t="s">
         <v>31</v>
       </c>
@@ -2404,7 +2404,7 @@
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="9"/>
+      <c r="A87" s="15"/>
       <c r="B87" s="3" t="s">
         <v>94</v>
       </c>
@@ -2417,7 +2417,7 @@
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="9"/>
+      <c r="A88" s="15"/>
       <c r="B88" s="2" t="s">
         <v>95</v>
       </c>
@@ -2430,7 +2430,7 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" s="9"/>
+      <c r="A89" s="15"/>
       <c r="B89" s="2" t="s">
         <v>96</v>
       </c>
@@ -2443,7 +2443,7 @@
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="9"/>
+      <c r="A90" s="15"/>
       <c r="B90" s="2" t="s">
         <v>97</v>
       </c>
@@ -2456,7 +2456,7 @@
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="9"/>
+      <c r="A91" s="15"/>
       <c r="B91" s="2" t="s">
         <v>98</v>
       </c>
@@ -2469,7 +2469,7 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="9"/>
+      <c r="A92" s="15"/>
       <c r="B92" s="2" t="s">
         <v>99</v>
       </c>
@@ -2482,7 +2482,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A93" s="9"/>
+      <c r="A93" s="15"/>
       <c r="B93" s="3" t="s">
         <v>100</v>
       </c>
@@ -2495,7 +2495,7 @@
       </c>
     </row>
     <row r="94" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A94" s="9"/>
+      <c r="A94" s="15"/>
       <c r="B94" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>